<commit_message>
Added final speeches of 2021.
</commit_message>
<xml_diff>
--- a/_data/Prednasky_2017.xlsx
+++ b/_data/Prednasky_2017.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="100" windowWidth="38340" windowHeight="18090"/>
+    <workbookView xWindow="80" yWindow="100" windowWidth="38340" windowHeight="18090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prednasky_2017_2" sheetId="1" r:id="rId1"/>
+    <sheet name="Prednasky_2021" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="336">
   <si>
     <t>Prednasejici</t>
   </si>
@@ -736,12 +737,991 @@
   <si>
     <t>Jak se snažím praktikovat hlubokou práci a co mi při tom pomáhá.</t>
   </si>
+  <si>
+    <t>Kvantové počítače</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pA8a0nLdKlU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;využívá se znalostí quantové mechaniky&lt;ul&gt;
+&lt;li&gt;suprapozice, &lt;/li&gt;
+&lt;li&gt;interference - mohou se zvýraznit a &lt;/li&gt;
+&lt;li&gt;entanglement - schopnost provázat dvě částice geograficky vzdálené&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;umožňují řešit exponenciálně ryhchleji problémy neřešitelné jiným způsobem&lt;ul&gt;
+&lt;li&gt;RSA šifra - Shorův algoritmus &lt;/li&gt;
+&lt;li&gt;kdy bude prolomen bitcoin? &lt;/li&gt;
+&lt;li&gt;výzkum materiálů - sloučenin, které jsou možné je velké množství, které není ani možné vyzkoušet a kvantové počítače mohou být velmi efektivní v simulaci&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;hlavní problém - extrémní fyzikální podmínky a s tím spojený šum&lt;ul&gt;
+&lt;li&gt;velký pokrok v posledních letech&lt;/li&gt;
+&lt;li&gt;odhad že za deset let dojde k velkému zlomu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;kvantové obvody&lt;ul&gt;
+&lt;li&gt;u klasických obvodů máme hradla&lt;/li&gt;
+&lt;li&gt;kvanmtové obvody jsou obecnější - vstupy a výstupy nemusí být jen 0 / 1, uvažuje se superpozice
+měření p zmizení superpozice se převede na 0,1&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;kvantový stav qbitu &lt;ul&gt;
+&lt;li&gt;představa koule v prostoru, severní pól 9, jižný 1, a každý bod na této svéře je validným stavem.&lt;/li&gt;
+&lt;li&gt;tento bot je možné vyjádřit dvojicí komplexních čísel&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;kvantové hradlo &lt;ul&gt;
+&lt;li&gt;násobí unitární maticí - abysme se stále pohybovali po povrchu koule ve validním stavu&lt;/li&gt;
+&lt;li&gt;pauliho-X hradlo&lt;/li&gt;
+&lt;li&gt;NOT &lt;/li&gt;
+&lt;li&gt;CX - CNOT hradlo&lt;ul&gt;
+&lt;li&gt;kontrolované hradlo, dva vstupy dva výstupy&lt;/li&gt;
+&lt;li&gt;jeden vstup je kontolní - pracuje jen když je na něm jednička&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Halamardovo hradlo &lt;ul&gt;
+&lt;li&gt;transformuje dva stavy do superpozice&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Kvantový Hello World -sestavení obvodu&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Spuštění - na simulátoru, nebo na kvantovém počítači&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;typicky se spouští mnohorkát kvůli šumu - aby statisticky vygeneroval správný výsledek
+spuštění na kvantovém počítači&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;dostupný prakticky zadarmo v každém cloudu&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;praktický příklad použití je bezpečnost a kryptografie&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>ZX Spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;23.dubna 2022 - výročí 40 let&lt;/li&gt;
+&lt;li&gt;počítač se nerozpadl v prach, komunita nespí a vyrábí se klony&lt;/li&gt;
+&lt;li&gt;v osobním volnu dělá vývoj na spectru&lt;/li&gt;
+&lt;li&gt;má doma krásné muzeum ZX techniky a originálnho SW&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Čím to začalo &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;23.dubna - 1982&lt;/li&gt;
+&lt;li&gt;ZX Spectrum - Sir Clive Sinclair&lt;/li&gt;
+&lt;li&gt;30.7. 1944 - 16.9. 2021&lt;/li&gt;
+&lt;li&gt;Didaktik Gama&lt;/li&gt;
+&lt;li&gt;Didaktik M - nejstabilnější klon&lt;/li&gt;
+&lt;li&gt;Kompakt - s didketovkou&lt;/li&gt;
+&lt;li&gt;90 léta - usnulo - na smetišti zadarmo&lt;/li&gt;
+&lt;li&gt;Ben Heck - ZX Spectrum na nepájivém poli&lt;/li&gt;
+&lt;li&gt;poměrně jednoduché&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Dnes jak se dělají&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Diskrétní součástky - old school, velký problém s ula chipem&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Harlequin 128 - stavebnice z didkrétních součástek &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;softwarová emulace - neemulují rozšiřující sběrnici&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;v system on chip vytvořená Spectrum emulace&lt;/li&gt;
+&lt;li&gt;VEGA - krabička která se připojí k televizi &lt;/li&gt;
+&lt;li&gt;ZX Baremulator - raspberry pi emulator&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;FPGA&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;100% kompatibilní se Spectrem ale drahé&lt;/li&gt;
+&lt;li&gt;ZX spectrum next - krásné zařízení ale nedostupné&lt;/li&gt;
+&lt;li&gt;Překvapivě velká komunita&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Oldcomp.cz&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Bytefest 2021 konference v Praze&lt;/li&gt;
+&lt;li&gt;ZX Spectrum a Kamilovy projekty&lt;/li&gt;
+&lt;li&gt;TV digitizer - Cinch composite - HDMI&lt;/li&gt;
+&lt;li&gt;Plošinovka Dizzy - v Kotlinu&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1fJy3fzri-M</t>
+  </si>
+  <si>
+    <t>Jak vyhrát diskusi na internetu</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pu6e2Dlh0hQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;Zesměšnit &lt;/li&gt;
+&lt;li&gt;Ukázat fakta&lt;/li&gt;
+&lt;li&gt;Nenásilná cesta - &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Co vyvolává nepravda  na internetu - emoce - zlost frustraci&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;vztek = strach / stud / bezmoc&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Postup &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;ubrzdit automatickou reakci&lt;/li&gt;
+&lt;li&gt;pochopit svoje pocity - proč mi to vadí&lt;/li&gt;
+&lt;li&gt;pochopit co potřebuje ten druhý&lt;/li&gt;
+&lt;li&gt;pobavit se o tom jak to udělat spolu&lt;/li&gt;
+&lt;li&gt;&lt;a href="https://nenasilnakomunikace.org/"&gt;https://nenasilnakomunikace.org/&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Kartičky&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;stěžejní pomůžou pojmenovat svoje emoce&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Martin Talpa</t>
+  </si>
+  <si>
+    <t>Life 3.0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/3hj8nIFKHPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;možný vliv umělé inteligence na lidskou společnost&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Co je život? &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;život → kultura (změna vlastního SW) → technologický život (změna vlastního SW i HW)&lt;/li&gt;
+&lt;li&gt;Inteligence - schopnost řešit komplikované tasky&lt;/li&gt;
+&lt;li&gt;dnes vídáme spíše slabou AI - šachy - ale neumí řídit auto&lt;/li&gt;
+&lt;li&gt;obecná inteligence - schopnost řešit jakýkoli problém stejně jako člověk&lt;/li&gt;
+&lt;li&gt;Superinteligence - za hranicemi člověka&lt;/li&gt;
+&lt;li&gt;Inteligence Explosion - inteligence, která se dokáže vylepšovat&lt;/li&gt;
+&lt;li&gt;Kniha Life 3.0 - Max Tegmark &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Hypotetická situace 
+1 - systém umí generovat AI systémy a vylepšovat se
+2 - během dne sám sebe vylepší a může vydělávat peníze bude řešit MTurk tasky ty dojdou
+kam dál - počítačové hry a programy ne - co kdyby vytvořil něco nebezpečného 
+3 - filmy - přečte knihy, scénáře a začne psát filmy a vydělá víc než všichni dohromady
+4 - Nestačí AWS- začne designovat datacentra aby měl kde běžet
+5 - získání moci &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;média - generování textu a analýza politické situace&lt;/li&gt;
+&lt;li&gt;ví jak podpořit, a koho se zbavit pomocí&lt;/li&gt;
+&lt;li&gt;pokud mají nejčtenější média tak je to velmi jednoduché nejsou zlí
+6 - nový svět - AI vybírá to nejlepší pro lidskou společnost a podporuje, tím vzniká víc stejně smýšlejících stran a lidé je podporují
+7 - aliance přeroste i vlády a na pozadí bude ovládat celý svět
+lidé jsou spokojení, protože všechno funguje dobře&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Milan Lempera</t>
+  </si>
+  <si>
+    <t>XTDB - CruxDb</t>
+  </si>
+  <si>
+    <t>https://youtu.be/v0T4aOaadoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;svět funguje v čase a často si jej zjednodušujeme&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Např:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;objednávkový systém&lt;/li&gt;
+&lt;li&gt;adresa odběratele se mění ale chceme mít historické hodnoty&lt;/li&gt;
+&lt;li&gt;evidence zaměstandů&lt;ul&gt;
+&lt;li&gt;mění se jména, náklady&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Bitemporal databáze&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;v databázi jsou dva zaznamy o čase&lt;/li&gt;
+&lt;li&gt;valid time, transaction time, decision time&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Použití XTDB&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;transakce - put / delete / match /evict&lt;/li&gt;
+&lt;li&gt;přistupuje se k jsonu&lt;/li&gt;
+&lt;li&gt;dotazuje se pomocí datalogu&lt;/li&gt;
+&lt;li&gt;dotazy dle času ukazují aktuální stav&lt;/li&gt;
+&lt;li&gt;evict - umožní zapomenout - řešení gdpr&lt;/li&gt;
+&lt;li&gt;SQL adapter  - pokud nevyhovuje datalog je možné sql&lt;/li&gt;
+&lt;li&gt;Java API, HTTP api&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Dotaz do publika - jak toto řešíte:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;duplikace dat - bobtnání dat&lt;/li&gt;
+&lt;li&gt;vložení kopie (adresa do objednávky)&lt;/li&gt;
+&lt;li&gt;datový sklad - protože v realtimu není historie často třeba&lt;/li&gt;
+&lt;li&gt;workspace - v oraclu&lt;/li&gt;
+&lt;li&gt;datalog umožňuje doptávat se na logické vazby (jméno herce, který hrál s vybraným hercem a je mladší než on)&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Petr Filip</t>
+  </si>
+  <si>
+    <t>Jak jsem programoval RT multiplayer hru</t>
+  </si>
+  <si>
+    <t>https://youtu.be/EC8ip3jqpgk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;z programátorského hlediska nutno vyřešit, jak komunikovat&lt;/li&gt;
+&lt;li&gt;jaká data posílat na a z klienta&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Přenos dat&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;long pooling - spousta requestů / responsů&lt;/li&gt;
+&lt;li&gt;event source - data jen ke klientovi&lt;/li&gt;
+&lt;li&gt;websockety - obousměrná komunikace&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;nejdůležitější je samotný stav - &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;GameState = (currentState, moves, rules) = rules(currentState, moves)&lt;/li&gt;
+&lt;li&gt;ukládal historii stavu pro možnost znovuposlání - je k ničemu&lt;/li&gt;
+&lt;li&gt;ale poté došlo k tomu, že se posílal stále celý stav &lt;/li&gt;
+&lt;li&gt;v nové hře potřebujete&lt;/li&gt;
+&lt;li&gt;vykreslovací vrstva&lt;/li&gt;
+&lt;li&gt;definice stavu hry&lt;/li&gt;
+&lt;li&gt;pravidla&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Tomáš Látal</t>
+  </si>
+  <si>
+    <t>Parse, don´t validate</t>
+  </si>
+  <si>
+    <t>https://youtu.be/KbRXQKzmoZU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;funkcionální přístup umožní odstranit validaci vstupu z funkcí&lt;/li&gt;
+&lt;li&gt;pomocí parseru můžete z méně strukturovaného vstupu udělat více strukturovaný&lt;/li&gt;
+&lt;li&gt;dovnitř funkcí se pustí validní vstupy, nad kterými nemusíte dělat žádné kontroly&lt;/li&gt;
+&lt;li&gt;silný vstupní typ, slabý výstupní typ&lt;/li&gt;
+&lt;li&gt;neprázdné pole&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;neduplicitní pole&lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;může vést k tomu, že nevalidní data se protáhnou systémem, a až na konci se zjistí, že nevyhovuje
+v Elmu na to ale příjde při kompilaci &lt;/p&gt;
+&lt;/li&gt;
+&lt;li&gt;možnost zapouzdřit třeba číslo karty, kde nikde neuteče číslo a bude zde jen poslední čtveřice&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Lego</t>
+  </si>
+  <si>
+    <t>https://youtu.be/lLITLwRRlts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;pokud máte sety z lega, často děti vyžadují další sety což není příliš ekologické a leze to do peněz&lt;/li&gt;
+&lt;li&gt;služba rebrickable - návody na alternativní plány pro sety z lega&lt;/li&gt;
+&lt;li&gt;podle čísel setů umožňuje vyhledat a stáhnout návody na řadu dalších modelů ze setů, které už máte&lt;/li&gt;
+&lt;li&gt;je možné si vytvořit jednoduchou bluetooth klávesnici na tři tlačítka s cenou 250 Kč, stačí umět trochu pájet&lt;/li&gt;
+&lt;li&gt;doporučuje nahrávat s dětmi návody na složení modelů pomocí stop motion aplikací v mobilu / tabletu&lt;/li&gt;
+&lt;li&gt;bricklink, umožňuje najít konkrétní dílek, který se ztratil a najít obchody, které je prodávají a v Čechách jich je hodně. Dílek stačí často třeba jen korunu.&lt;/li&gt;
+&lt;li&gt;IKEA příborník se hodí na kategorizaci dílků lega podle typu&lt;/li&gt;
+&lt;li&gt;třídit lze dobře ručně quicksortem&lt;/li&gt;
+&lt;li&gt;na YT je i video, které představuje automatickou třídičku, která používá AI na třídění dílků lega - &lt;a href="https://www.youtube.com/watch?v=04JkdHEX3Yk&amp;amp;ab_channel=DanielWest"&gt;https://www.youtube.com/watch?v=04JkdHEX3Yk&amp;amp;ab_channel=DanielWest&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Strudio pro design lego modelů - &lt;a href="https://www.bricklink.com/v3/studio/download.page"&gt;https://www.bricklink.com/v3/studio/download.page&lt;/a&gt;
+Brickling - bible lega - &lt;a href="https://www.bricklink.com/v2/main.page"&gt;https://www.bricklink.com/v2/main.page&lt;/a&gt; 
+Rebrickable - alternativní modely - &lt;a href="https://rebrickable.com/home/"&gt;https://rebrickable.com/home/&lt;/a&gt;&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>https://youtu.be/A85Fvn2gQSA</t>
+  </si>
+  <si>
+    <t>AsciiiDoc a PlantUML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;ASCII doc je principem podobný markdownu, ale hodí se na psaní celých knih&lt;/li&gt;
+&lt;li&gt;má rozšíření pro poznámky, sidebary, poznámky pod čarou, citace, zdrojový kód&lt;/li&gt;
+&lt;li&gt;jeden z pluginů je PlantUML, který umí activity diagramy, sekvenční, deployent diagramy, vizualizovat JSON … velmi jednoduše se ty diagramy píší&lt;/li&gt;
+&lt;li&gt;výsledkem je velmi produktivní a spravovatelná dokumentace&lt;/li&gt;
+&lt;li&gt;nevýhody - klient to nemůže editovat - komentáře jen jako code review, diagramy nelze doladit o layoutu rozhoduje algoritmus, při větším množství obrázků je to pomalejší&lt;/li&gt;
+&lt;li&gt;výhody: lze to verzovat, rozdělit a includovat&lt;/li&gt;
+&lt;li&gt;formát umožňuje plno věcí a zároveň není výsledek rozbitý, formát je robustní&lt;/li&gt;
+&lt;li&gt;dokumentace se builduje Mavenem, existuje plugin do IntelliJ Idea … musí se ale něco doinstalovávat na stroj, který provádí publikaci&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Vojtěch Růžička</t>
+  </si>
+  <si>
+    <t>Web monetization</t>
+  </si>
+  <si>
+    <t>https://youtu.be/s1pOmM6J1u8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;pokud jsem tvůrce na webu a chci platit&lt;ul&gt;
+&lt;li&gt;reklamy&lt;/li&gt;
+&lt;li&gt;paywall - zaplaťte pro další čtení&lt;/li&gt;
+&lt;li&gt;jsou velmi invazivní&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Brave browser &lt;ul&gt;
+&lt;li&gt;řeší privacy&lt;/li&gt;
+&lt;li&gt;řeší odměňování tvůrců&lt;/li&gt;
+&lt;li&gt;za reklamu dostávám BAT Cryptocurrency&lt;/li&gt;
+&lt;li&gt;na stránce vidím, zda stránka může získávat odměnu&lt;/li&gt;
+&lt;li&gt;můžu poslat přímo&lt;/li&gt;
+&lt;li&gt;můžu nastavit auto příspěvek - podle toho, jak na web chodím.&lt;/li&gt;
+&lt;li&gt;po spárování peněženky, mohu jako tvůrce dostávat odměnu&lt;/li&gt;
+&lt;li&gt;podpora také github, youtube, reddit, twitter, umožňuje odměňovat  &lt;/li&gt;
+&lt;li&gt;problém - svázáno s prohlížečem - aktuálně 38M uživatelů&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Web Monetization - návrh standardu W3C&lt;ul&gt;
+&lt;li&gt;po schválení by mohli podporovat prohlížeče&lt;/li&gt;
+&lt;li&gt;Uživatel&lt;ul&gt;
+&lt;li&gt;Registruju se u poskytovatele - platím Coil - (5$ měsíc&lt;/li&gt;
+&lt;li&gt;Aktuálně není standard - tedy potřebuju plugin&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Poskytovatel&lt;ul&gt;
+&lt;li&gt;Registrace&lt;/li&gt;
+&lt;li&gt;připojení peněženky - Gatehub / uphold&lt;/li&gt;
+&lt;li&gt;JS api, můžu se dotazovat na eventy (začal platit)&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Aktuálně Web Monetization menší použití než Brave Browser&lt;/li&gt;
+&lt;li&gt;API aktuálně nepodporuje “subscription” spíše funguje stylem, kudy chodím, tudy trousím peníze&lt;/li&gt;
+&lt;li&gt;dev.to - integruje&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Zbyšek Voda</t>
+  </si>
+  <si>
+    <t>Jak na desky plošných spojů</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4P1EIzeJ9m8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;v čem navrhovat:&lt;ul&gt;
+&lt;li&gt;EasyEDA - online, napojeno na prodejce součástek, jednoduše se vyrobí tišťák&lt;/li&gt;
+&lt;li&gt;KiCad - oblíbený - opensource, stojí za ním CERN&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Kroky návrhu&lt;ul&gt;
+&lt;li&gt;Schéma&lt;/li&gt;
+&lt;li&gt;Konkrétní součástky&lt;/li&gt;
+&lt;li&gt;Import tvaru výsledné desky - vrstva - edge cuts&lt;/li&gt;
+&lt;li&gt;Rozmístění součástek&lt;/li&gt;
+&lt;li&gt;Nakreslení spojů&lt;/li&gt;
+&lt;li&gt;Vygenerování jednotlivých vrstev pro tvorbu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Výběr výrobce&lt;ul&gt;
+&lt;li&gt;číňan&lt;/li&gt;
+&lt;li&gt;Pragoboard&lt;/li&gt;
+&lt;li&gt;Isler&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;ukázka objednávky - JLCPCB&lt;ul&gt;
+&lt;li&gt;upload a výběr barev&lt;/li&gt;
+&lt;li&gt;naklikám&lt;/li&gt;
+&lt;li&gt;za 14 dní + celní řízení a mám je doma&lt;/li&gt;
+&lt;li&gt;je možné obědnat i se součástkama - KiCad by měl umět PCBA (PCB assembly)&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Jak (vy)řešíme GDPR</t>
+  </si>
+  <si>
+    <t>https://youtu.be/h-jldaLcUsY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;osobní údaj je v principu cokoliv podle čeho je možné identifikovat&lt;ul&gt;
+&lt;li&gt;možnost nakládat ukládá zákon, oprávněný zájem, souhlas&lt;/li&gt;
+&lt;li&gt;požadavky zákazníka&lt;/li&gt;
+&lt;li&gt;mít zákazníka jednou, se správnou rolí&lt;/li&gt;
+&lt;li&gt;historizace&lt;/li&gt;
+&lt;li&gt;omezená viditelnost, (pseudo)anonymizace&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;architektura&lt;ul&gt;
+&lt;li&gt;IDM - zná jen identifikátor, nezná email uživatele - &lt;/li&gt;
+&lt;li&gt;při přihlášení emailem se vytvoří hash proti kterému se porovnává&lt;/li&gt;
+&lt;li&gt;rejstřík osob pro osobní údaje - ta drží osobní data&lt;/li&gt;
+&lt;li&gt;profily - implementace role s daty navíc&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;REST API&lt;ul&gt;
+&lt;li&gt;zámky - data nelze měnit, musí udělat externí autorita, nebo právní zákaz změny dat&lt;/li&gt;
+&lt;li&gt;vše v paměti&lt;/li&gt;
+&lt;li&gt;úložiště ala firebase, event- driven úpravy&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Kde je to GDPR?&lt;ul&gt;
+&lt;li&gt;data na jednom místě&lt;/li&gt;
+&lt;li&gt;klienti pracují jen s ID + displayName&lt;/li&gt;
+&lt;li&gt;anonymizace na jednom místě v kombinaci se zámky&lt;/li&gt;
+&lt;li&gt;auditní stopa&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Audit a startup</t>
+  </si>
+  <si>
+    <t>https://youtu.be/_5uYw4ARMnA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;i v prostředí startupu se dá s auditem vyrovnat&lt;ul&gt;
+&lt;li&gt;chtějí vědět co děláte a co bude když se to rozsype&lt;/li&gt;
+&lt;li&gt;auditoři mají rozum a do malého týmu tolik netlačí&lt;/li&gt;
+&lt;li&gt;zpřesňování auditu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;PCI-DSS - práce s platebními kartami  &lt;ul&gt;
+&lt;li&gt;Roční KPMG audit&lt;/li&gt;
+&lt;li&gt;Due Diligence&lt;/li&gt;
+&lt;li&gt;2 týdny práce pro několik lidí&lt;/li&gt;
+&lt;li&gt;spousta otázek z jiného světa &lt;/li&gt;
+&lt;li&gt;dopisován dokumentace&lt;/li&gt;
+&lt;li&gt;dohledávání &lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Nejvíc je zajímá &lt;ul&gt;
+&lt;li&gt;Change management&lt;/li&gt;
+&lt;li&gt;github + youtrack stačil&lt;/li&gt;
+&lt;li&gt;Důležité mít malý počet lidí, kteří mohou zasahovat do produkce&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Vše zaznamenávat&lt;ul&gt;
+&lt;li&gt;Mít penetrační testy - auditorům stačí mít zaškrtnuto, že mají&lt;/li&gt;
+&lt;li&gt;Pci-DSS&lt;/li&gt;
+&lt;li&gt;nemít citlivá data a mít oddělené služby&lt;/li&gt;
+&lt;li&gt;Dodavatel měl jednoduchou databázi Key value - prodával za těžké peníze, protože procházel audity &lt;/li&gt;
+&lt;li&gt;není třeba splnit vše&lt;/li&gt;
+&lt;li&gt;nelhat a přiznat, že něco neumíme, je na majitelých aby se rozhodli co s tím&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Guix</t>
+  </si>
+  <si>
+    <t>https://youtu.be/qtUdGQe2O7Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;výběr distribuce linuxu&lt;/li&gt;
+&lt;li&gt;ubuntu, debian - nuda, používají to všichni&lt;/li&gt;
+&lt;li&gt;GUIX - distribuce a package manager&lt;ul&gt;
+&lt;li&gt;Balíčkovací manager&lt;/li&gt;
+&lt;li&gt;zajišťují verzování souborů&lt;/li&gt;
+&lt;li&gt;řeší závislosti balíčků - nedovolí mít více balíčků ve stejné verzi&lt;/li&gt;
+&lt;li&gt;breaking update - nemůžu mít knihovny, které závisí na různých verzích &lt;/li&gt;
+&lt;li&gt;musím potenciálně upgradovat když nechci, nebo musím počkat na upgrade&lt;/li&gt;
+&lt;li&gt;je těžké zreplikovat instalaci současného systému&lt;/li&gt;
+&lt;li&gt;některé balíčky mohou být novější&lt;/li&gt;
+&lt;li&gt;při použití více balíčkovacích systémů musíme řešit kompilaci&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;GUIX&lt;ul&gt;
+&lt;li&gt;umožní mít balíčky ve více verzích &lt;/li&gt;
+&lt;li&gt;při instalaci vytváří profil a ukládá s hashem a zachovává starou verzi balíčku&lt;/li&gt;
+&lt;li&gt;profil - skupina balíčků&lt;/li&gt;
+&lt;li&gt;balíčky mohou být z libovolné doby - je možné replikovat jakýkoli stav&lt;/li&gt;
+&lt;li&gt;channel - repository s definicemi balíčků, commit určuje verze všech balíčků &lt;/li&gt;
+&lt;li&gt;source code distribuce - s binárními substitute&lt;/li&gt;
+&lt;li&gt;GNU - libre kernel - nemá svobodné balíčky&lt;/li&gt;
+&lt;li&gt;Asdf - možnost mít více verzí runtimu a přepíná podle adresářů - &lt;a href="https://github.com/asdf-vm/asdf"&gt;https://github.com/asdf-vm/asdf&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>K čemu je pravda</t>
+  </si>
+  <si>
+    <t>https://youtu.be/hRycaM3mfAk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;Samoopravné a samodetekující kódy &lt;ul&gt;
+&lt;li&gt;pokud posíláme po nespolehlivém kanálu &lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;řešení&lt;ul&gt;
+&lt;li&gt;zdvojení - samodetekující kód - nezjistíme ale co je správně&lt;/li&gt;
+&lt;li&gt;ztrojení - samoopravný - pravděpodobně opravíme podle dvou správných&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Hammingův kód&lt;ul&gt;
+&lt;li&gt;4 bity zakódujeme pomocí 7 kódů&lt;/li&gt;
+&lt;li&gt;vypočítá se “syndrom” - zjistí chybu v konkrétním bitu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Kompilátor&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;v kódu má dostatek redundance na to, aby vydedukoval co jsme chtěli udělat&lt;/li&gt;
+&lt;li&gt;navlékáme kód na syntaxi&lt;/li&gt;
+&lt;li&gt;pokud je kód složitý a není tam dostatek redundance, tak není možné zjistit kde je chyba - například Java Streamy&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Explicitní tvrzení o skutečnosti jsou redundantní&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;pravdivé tvrzení může sloužit jako kontrolní redundance&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;V programování -Curry-Howardova korespondence&lt;ul&gt;
+&lt;li&gt;datový typ odpovídá logicky dokazovanému tvrzení a program je jeho důkaz&lt;/li&gt;
+&lt;li&gt;Redundance v programovacím jazyce je tradeoff&lt;/li&gt;
+&lt;li&gt;je třeba vyměnit výhody na nevýhody&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Evita DB</t>
+  </si>
+  <si>
+    <t>https://youtu.be/lPOKjeAwaXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;E-commerce API pro sjednocení frontendů e-shopů&lt;ul&gt;
+&lt;li&gt;důraz na rychlost&lt;/li&gt;
+&lt;li&gt;google preferuje rychlé odezvy&lt;/li&gt;
+&lt;li&gt;research grant&lt;/li&gt;
+&lt;li&gt;tři konkurenční týmy&lt;/li&gt;
+&lt;li&gt;standardizované api&lt;/li&gt;
+&lt;li&gt;tři implementace - PostgreSQL / Elasticsearch / in-memory noSQL - &lt;/li&gt;
+&lt;li&gt;FG forrest se zabývá in-memory databází&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;kritéria&lt;ul&gt;
+&lt;li&gt;kompletní api&lt;/li&gt;
+&lt;li&gt;rychlost&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Zajímavé knihovny&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Roaring Bitmaps&lt;ul&gt;
+&lt;li&gt;práce s rozsáhlýma polema čísel (ID záznamy v databázi) &lt;/li&gt;
+&lt;li&gt;automaticky kombinuje pole, BitSet , run-length encoding&lt;/li&gt;
+&lt;li&gt;velká úspora proti výběru pouze jedné strategie - pro každý případ se použije nejvýhodnější varianta&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Kryo - serializační knihovna&lt;ul&gt;
+&lt;li&gt;řeší pomalost standardní serializace&lt;/li&gt;
+&lt;li&gt;1,5gb dat - 7 sekund&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Random testing&lt;ul&gt;
+&lt;li&gt;testování náhodných operací nad datovými strukturami&lt;/li&gt;
+&lt;li&gt;používá pro transaction memory&lt;/li&gt;
+&lt;li&gt;porovnávání operací nad referenční implementací a vlastní implementací&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Výkonostní testy&lt;ul&gt;
+&lt;li&gt;CI/CD job - vytvoří infrastructure nad digital ocean,  spustí testy a pošlou do gistu a infrastruktura se zruší - nízká cena&lt;/li&gt;
+&lt;li&gt;JMH - visualiser - zobrazuje JSON z Gistu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Jaromír Pešout</t>
+  </si>
+  <si>
+    <t>Shenandoah GC</t>
+  </si>
+  <si>
+    <t>https://youtu.be/FEjtThV3gao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;firma Luxonit - low latency Java - zpracování dat&lt;ul&gt;
+&lt;li&gt;Ve finančním světě se dělají aplikace v C++ kvůli absenci garbage projektoru&lt;/li&gt;
+&lt;li&gt;díky nízké latency by bylo možné problém považovat za vyřešený&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Shenandoah GC&lt;ul&gt;
+&lt;li&gt;JDK 8 - 17&lt;/li&gt;
+&lt;li&gt;low pause time&lt;/li&gt;
+&lt;li&gt;negenerační kolektor&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Cyklus shenandoah&lt;ul&gt;
+&lt;li&gt;Konkurenční fáze -  s aplikací Continuous mark&lt;/li&gt;
+&lt;li&gt;Paralelní fáze&lt;/li&gt;
+&lt;li&gt;Celá halda se prohledává najednou&lt;/li&gt;
+&lt;li&gt;pauza závislá na velikosti root setu - 5-10%&lt;/li&gt;
+&lt;li&gt;vysoké nároky na paměť, ideální utilizace 30%&lt;/li&gt;
+&lt;li&gt;poté zpomalení a prodloužení pauzy&lt;/li&gt;
+&lt;li&gt;Amazon corretto pracuje na podpoře generací &lt;/li&gt;
+&lt;li&gt;JDK 16-17 - concurent stack processing&lt;/li&gt;
+&lt;li&gt;STW méně než 1 ms&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Výuka programování bez PC</t>
+  </si>
+  <si>
+    <t>https://youtu.be/6HcTuM3P0Aw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;ve volném čase vede kroužek programování&lt;ul&gt;
+&lt;li&gt;jako první věc chce naučit převod z 10ky do 2kové&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;jako v Hejného matematice&lt;ul&gt;
+&lt;li&gt;základní schopnost - rozpoznávání vzorců opakování&lt;/li&gt;
+&lt;li&gt;trénovat barvy, nebo geometrické tvary&lt;/li&gt;
+&lt;li&gt;iq testy jsou pěkné úlohy na opakování&lt;/li&gt;
+&lt;li&gt;trendem jsou bloková schémata &lt;/li&gt;
+&lt;li&gt;úloha s podmínkami a kratami &lt;/li&gt;
+&lt;li&gt;rychle se naučí sledovat kroky, ale problém je abstrakce a opakování&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;datová struktura algoritmů&lt;ul&gt;
+&lt;li&gt;komprese &lt;ul&gt;
+&lt;li&gt;zvládne i druhá třída&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;kontrolní číslice - čárový kód&lt;/li&gt;
+&lt;li&gt;třídění &lt;ul&gt;
+&lt;li&gt;děti podle schématu mohou putovat v políčcích a na konci budou seřazení&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;grafové algoritmy &lt;ul&gt;
+&lt;li&gt;spojení mezi městečky&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Bobřík informatiky - spousta úkolů pro různé věkové kategorie&lt;/li&gt;
+&lt;li&gt;Podzimní aktivita Codeweek&lt;/li&gt;
+&lt;li&gt;Stavebnice&lt;ul&gt;
+&lt;li&gt;Boffin a klony&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Důležitost komunikace&lt;ul&gt;
+&lt;li&gt;pomocí lega a tiché pošty je možné tvořit stavby, a porovnávat se zadáním - dobrá ukázka, že komunikace je důležitá&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Turring Tumble - turingtumble.com &lt;ul&gt;
+&lt;li&gt;turingovský počítač&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Tomáš Záluský</t>
+  </si>
+  <si>
+    <t>Neo4j</t>
+  </si>
+  <si>
+    <t>https://youtu.be/AyaAB8rcl3Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;grafová databáze&lt;ul&gt;
+&lt;li&gt;subset Cetin Network Inventory - 140 000 uzlů, 1.5M hran&lt;/li&gt;
+&lt;li&gt;úloha - analýza výpadků v síti&lt;/li&gt;
+&lt;li&gt;původní implementace - oracle &lt;/li&gt;
+&lt;li&gt;v nové implementaci - zmenšení datového skladu a napojení na Neo4j&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;přechod mezi paradigmaty&lt;ul&gt;
+&lt;li&gt;řádek možno připodobnit k uzlu v grafu&lt;/li&gt;
+&lt;li&gt;relationship není přímo hrana ale je to jemnější propojení &lt;/li&gt;
+&lt;li&gt;nemusí odpovídat 1:1&lt;/li&gt;
+&lt;li&gt;dotazuje se jazykem Cypher&lt;/li&gt;
+&lt;li&gt;grafové paradigma je silné pro hierarchie &lt;/li&gt;
+&lt;li&gt;je možné říct, kolikrát je možné přeskočit uzel&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;algoritmy a*&lt;ul&gt;
+&lt;li&gt;více se ptáme jak než co&lt;/li&gt;
+&lt;li&gt;java plugin - uložené procedury&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;netahejte skálu ke krumpáči.&lt;ul&gt;
+&lt;li&gt;Je možné vytvořit plugin do Neo4j, tedy vše se provádí v Neo4j&lt;/li&gt;
+&lt;li&gt;Traversal framework - umožní určit jak se graf bude procházet &lt;/li&gt;
+&lt;li&gt;dobrý sluha zlý pán&lt;/li&gt;
+&lt;li&gt;Plugin psali i kvůli zjednodušení, cypher by byl příliš složitý&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Databázi si hostuje cetin sám&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Zdeněk Henek</t>
+  </si>
+  <si>
+    <t>Volební obvody vytvořené genetickým algoritmem</t>
+  </si>
+  <si>
+    <t>https://youtu.be/WXHhkWAahK4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;změna pravidel vedla ke spravedlivějšímu rozdělení mandátů na hlasů&lt;/li&gt;
+&lt;li&gt;v 2017 - výsledky voleb vedly k tomu, že strany 6% měly 3% mandátů kvůli DHondtovu pravidlu&lt;/li&gt;
+&lt;li&gt;Pokud si začnete měnit volební obvody budete obviněni z Gerrymanderingu&lt;/li&gt;
+&lt;li&gt;V USA okrsek zvolen tak že vypadal jako salamander&lt;/li&gt;
+&lt;li&gt;většinový volební systém vede k tomu, že ten kdo vyhraje o procento dostává všechny mandáty&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Jaký systém by měl být spravedlivý &lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;středočeský kraj -milion 397 tisíc &lt;/li&gt;
+&lt;li&gt;Karlovarský 300 tisíc  &lt;/li&gt;
+&lt;li&gt;menší kraj generuje míň mandátů&lt;/li&gt;
+&lt;li&gt;Autoredistrict - pomocí genetického algoritmu vytvořeny volební obvody, které mají stejný počet voličů - tedy potenciálně stejné zastoupení&lt;/li&gt;
+&lt;li&gt;algoritmus to zvládne pro ČR s rozdílem desítek lidí&lt;/li&gt;
+&lt;li&gt;genetický algoritmus&lt;/li&gt;
+&lt;li&gt;pomocí fitness funkce zajistí spojitost okrsků &lt;/li&gt;
+&lt;li&gt;každý výpočet vypadá jinak&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Borek Bernard</t>
+  </si>
+  <si>
+    <t>Jak v JSONu poslat číslo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/RMxoRjON8WI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;&lt;p&gt;některé api - posílají string, některé number&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;problém s number a přesností&lt;/li&gt;
+&lt;li&gt;řešíme přenos - datové typy v JSONUI&lt;/li&gt;
+&lt;li&gt;cena je normální číslo&lt;/li&gt;
+&lt;li&gt;IEEE 754&lt;/li&gt;
+&lt;li&gt;používá každá platforma&lt;/li&gt;
+&lt;li&gt;Kolem čísel je spousta bludů&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;Argumentace: 1.7 se nedá vyjádřit přesně - výsledkem je 1.69 nebo 1.7&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;1,7 - double&lt;/li&gt;
+&lt;li&gt;uloženo jako 1.699999 ….. &lt;/li&gt;
+&lt;li&gt;printing = 1.7 a nikdy 1.69 &lt;/li&gt;
+&lt;li&gt;Tedy argumentace je špatná&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;p&gt;JSON jako celek je string&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;JSON number je bezpečný na přenos, ale ne počítání&lt;/li&gt;
+&lt;li&gt;Přenos jako string má také své problémy - 7.47 - je formátorvací rozhodnutí&lt;/li&gt;
+&lt;li&gt;Pro přenos Number OK, ale ne pro výpočty&lt;/li&gt;
+&lt;li&gt;pro výpočty decimal datový typ &lt;/li&gt;
+&lt;li&gt;spočítat a zaokrouhlit&lt;/li&gt;
+&lt;li&gt;V Javě do BigDecimal&lt;/li&gt;
+&lt;li&gt;při převádění - použít string a ne number&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Martin Bednář</t>
+  </si>
+  <si>
+    <t>Istio</t>
+  </si>
+  <si>
+    <t>https://youtu.be/vBFZFtVR8gs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;service mesh &lt;ul&gt;
+&lt;li&gt;konkurence Linkerd(málo možností), Consul (komerční)&lt;/li&gt;
+&lt;li&gt;Istio - intenzivní vývoj &lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Funkce&lt;ul&gt;
+&lt;li&gt;Automatický load balancing - HTTP, gRPC, Sockety&lt;/li&gt;
+&lt;li&gt;routing, retrie mezi servisami, circuit breaker&lt;/li&gt;
+&lt;li&gt;je možné pracovat s chybovostí service - FaultInjection&lt;/li&gt;
+&lt;li&gt;metriky, a logy&lt;/li&gt;
+&lt;li&gt;zabezpečení, Autentizace autorizace (ingres)&lt;/li&gt;
+&lt;li&gt;dostupná v cloudu&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Architektura s Istio&lt;ul&gt;
+&lt;li&gt;do každého konteineru přidá proxy envoy&lt;/li&gt;
+&lt;li&gt;služba s proxy komunikuje s HTTP&lt;/li&gt;
+&lt;li&gt;service spolu komunikují přes https - control plane je generuje a posílá do proxy&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;GUI&lt;ul&gt;
+&lt;li&gt;Kiali - vizualizace provozu a konfigurace istia&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;Budoucnost&lt;ul&gt;
+&lt;li&gt;B/G deployments - Canary deployments&lt;/li&gt;
+&lt;li&gt;WASM - filtery&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Překlad do SQL</t>
+  </si>
+  <si>
+    <t>https://youtu.be/bDEiOfwmxTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;vytváří systém pro zpracování dat - no code system&lt;ul&gt;
+&lt;li&gt;velké množství práce v paměti po natažení všech dat do paměti &lt;/li&gt;
+&lt;li&gt;možno vylepšit&lt;/li&gt;
+&lt;li&gt;řada problémů &lt;ul&gt;
+&lt;li&gt;joiny&lt;/li&gt;
+&lt;li&gt;indexy&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;funkce nekorespondují v db a aplikaci&lt;ul&gt;
+&lt;li&gt;snaha o přepis do sql - Snowflake v cloudu&lt;/li&gt;
+&lt;li&gt;aktuálně zkouší proti sqllite&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>Lubomir Petera</t>
+  </si>
+  <si>
+    <t>https://youtu.be/d8zHlhoUXcA</t>
+  </si>
+  <si>
+    <t>Spolehlivost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;jak špatná může být špatná prezentace&lt;ul&gt;
+&lt;li&gt;kritéria úspěchu&lt;/li&gt;
+&lt;li&gt;máme tendenci žít v černobílém světě&lt;/li&gt;
+&lt;li&gt;kdo si řekne “super mám 60% programu přeloženo a pak to spadlo”&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;faktory kvality - Spolehlivost - požadované funkce s požadovanou přesností&lt;ul&gt;
+&lt;li&gt;SLA&lt;/li&gt;
+&lt;li&gt;SLO&lt;/li&gt;
+&lt;li&gt;SLO&lt;/li&gt;
+&lt;li&gt;KPI&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;li&gt;jakou škálu použít pro hodnocení jak vhodné je UI&lt;ul&gt;
+&lt;li&gt;nic není černobílé, je dobré znát celou škálu&lt;/li&gt;
+&lt;li&gt;často v porovnání s jinými, to nemusí být tak špatná volba &lt;/li&gt;
+&lt;li&gt;&lt;a href="https://userinyerface.com/"&gt;https://userinyerface.com/&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
+    <t>https://calavera.info</t>
+  </si>
+  <si>
+    <t>https://fnx.io</t>
+  </si>
+  <si>
+    <t>dond.cz</t>
+  </si>
+  <si>
+    <t>www.intelis.cz</t>
+  </si>
+  <si>
+    <t>blog.lempera.cz</t>
+  </si>
+  <si>
+    <t>blog.zvestov.cz</t>
+  </si>
+  <si>
+    <t>www.vojtechruzicka.com</t>
+  </si>
+  <si>
+    <t>sedlakovi.org</t>
+  </si>
+  <si>
+    <t>vitaplsek.cz</t>
+  </si>
+  <si>
+    <t>https://www.dynatrace.com/</t>
+  </si>
+  <si>
+    <t>www.pesout.cz</t>
+  </si>
+  <si>
+    <t>https://twitter.com/borekb</t>
+  </si>
+  <si>
+    <t>https://tix.cz/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,6 +1874,14 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1193,7 +2181,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1236,15 +2224,22 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % – Zvýraznění1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % – Zvýraznění2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % – Zvýraznění3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1264,6 +2259,7 @@
     <cellStyle name="60 % – Zvýraznění5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60 % – Zvýraznění6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Celkem" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Hypertextový odkaz" xfId="42" builtinId="8"/>
     <cellStyle name="Chybně" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Kontrolní buňka" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Nadpis 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1580,7 +2576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1652,7 +2648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="130.5">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2401,4 +3397,462 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.54296875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="64" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="41" spans="4:4">
+      <c r="D41" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F13" r:id="rId3"/>
+    <hyperlink ref="E17" r:id="rId4" display="https://blog.novoj.net/"/>
+    <hyperlink ref="E16" r:id="rId5" display="https://calavera.info/"/>
+    <hyperlink ref="E10" r:id="rId6" display="https://fnx.io/"/>
+    <hyperlink ref="E13" r:id="rId7" display="http://dond.cz/"/>
+    <hyperlink ref="E20" r:id="rId8" display="http://www.intelis.cz/"/>
+    <hyperlink ref="E6" r:id="rId9" display="http://blog.lempera.cz/"/>
+    <hyperlink ref="E19" r:id="rId10" display="http://blog.zvestov.cz/"/>
+    <hyperlink ref="E11" r:id="rId11" display="http://www.vojtechruzicka.com/"/>
+    <hyperlink ref="E14" r:id="rId12" display="http://sedlakovi.org/"/>
+    <hyperlink ref="E9" r:id="rId13" display="http://vitaplsek.cz/"/>
+    <hyperlink ref="E25" r:id="rId14"/>
+    <hyperlink ref="E18" r:id="rId15" display="http://www.pesout.cz/"/>
+    <hyperlink ref="E22" r:id="rId16"/>
+    <hyperlink ref="E7" r:id="rId17"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Year 2024 - lectures
</commit_message>
<xml_diff>
--- a/_data/Prednasky_2017.xlsx
+++ b/_data/Prednasky_2017.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Prednasky_2017_2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Prednasky_2021" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Prednasky_2022" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Prednasky_2023" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Prednasky_2024" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="773">
   <si>
     <t xml:space="preserve">Prednasejici</t>
   </si>
@@ -2942,6 +2943,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;ul&gt; &lt;li&gt;kde je hranice, která dělí vědomé bytosti od nevědomých?&lt;/li&gt; &lt;li&gt;má LLM vědomí?&lt;/li&gt; &lt;li&gt;theory of mind &lt;ul&gt; &lt;li&gt;já mám vědomí a protože vy jste podobní jako já, tak usuzuji, že máte taky vědomí&lt;/li&gt; &lt;li&gt;děti &amp;gt;= 4 roky, zvířata&lt;/li&gt; &lt;/ul&gt; &lt;/li&gt; &lt;li&gt;problém je, že LLM prochází (částí?) testů Theory of mind&lt;/li&gt; &lt;li&gt;popis operace řešící epilepsii, kdy se přeruší corpus callosum a člověk žije se dvěma nezávislými polovinami mozku, které spolu nekomunikují &lt;ul&gt; &lt;li&gt;z některých testů se zdá, že po této operací existují ve hlavě 2 osobnosti&lt;/li&gt; &lt;/ul&gt; &lt;/li&gt; &lt;li&gt;revize teorie - možná nakonec nikdo nemá vědomí 🙂&lt;/li&gt; &lt;/ul&gt;
 &lt;li&gt;kde je hranice, která dělí vědomé bytosti od nevědomých?&lt;/li&gt;
@@ -2966,6 +2968,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">🙂</t>
     </r>
@@ -2975,6 +2978,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/li&gt;
 &lt;/ul&gt;</t>
@@ -3246,6 +3250,303 @@
   </si>
   <si>
     <t xml:space="preserve">https://youtu.be/BQx_AizSyik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavel Košťál </t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Jak nevyhořet v práci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Jak jsem dělal pohovor do Google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mastodonczech.cz/@krab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1vAPAkLOSTeKivvjCpFT8fGvTJnNMqksJ4q5yKX8FkQ0/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Prompt Injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1etgJfsgDy_LR3eNW1ArESDER-lq1Fasqyx7TH6Tcmog/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Rok s elektromobilem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1DjGQOEuifkzH4lVNIA1wUB5S0-N43iNjK8XBSdCIZ28/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 L. Casei Securitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/miloshavranek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1e2b5doe5V0wi0DlxOmBCOKHLKwsu4Q6riUDtTpqEX7o/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 DDD + Spring Modulith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cz.linkedin.com/in/jirkapinkas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1GtbMVHhNK7DrKEw4cKfzkKqt7AKRV2OWIUK-j-dEXPY/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Talisman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://witter.cz/@banterCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1Y0jf3tYs3yv6qJ__QW7WA8orRGsQeyf9/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filip Staffa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 React server components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1xukBVbrc6piYvDD_lllap9GmMxBucU4n4plrO7b5Two/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Spring AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.vojtechruzicka.com/about/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1V0S-XLpO79DJUz9FeOLH2YzY7D5eFlNiZSiq4mEJaJA/edit#slide=id.g3042c971e74_0_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan Novotný </t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Fly with Java Recorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://novoj.github.io/reveal.js/jopenspace2024.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Retrospektiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Zero Sugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1gw9-1-7JpieulzRNrkte2SnQtOwsFaYndec0jEomNsk/edit#slide=id.g2d3e48ff1ef_0_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Optimalizace domácnosti na spotové ceny elektřiny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1xk2bZjr_H16P_NBaKTibx-E1dODgjiNG5WSagivHtmQ/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Toki Pona: Jazyk dobra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1YzXB9UEiNi6RIlDg987zW6ah0sgjNYYLtuUZ-S7N5S0/edit#slide=id.p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 IntelliJ IDEA few advanced debugging features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/bugs84/idea-debugging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Zákony SW architektury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1N3zPUTr-eB2q34Avn7g-x1Jt7DVaiBWI_XiJgFVyF4w/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Václav Stolín </t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 povídání o integračním testování </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vaclav-stolin/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1Dz3IoOa8e8ENW-s3wzTjO3lgnoDL80Ua9Sip1gJl1xs/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Sex? Sex!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mastodon.social/@dondcz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1-FaHoEOYTGCGuU-N3a8Kv5Zs7-cHMHgWWuueAtdNles/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Adventury - My guilty pleasure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/vitaplsek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1lpEmMXVCthu0ryCtH4RNhIxSfHZdD9dR/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Vaadin Flow - Programátorské nebe frontendu pro Javisty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1Mn2zGT3l1hjI-unTH6ch7dGVGUJ8hg_K/edit?usp=sharing&amp;ouid=116470056523174499937&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Cloud Native Postgres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sika.io/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1zeEhah2i5J5RGENYm9ieA91JhK5lD3lwWQc0RU_Pa28/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 DX &gt; Cold Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1ZkpR4FWX_VRYsC-U6jDXRV5lwcpXd9ietQp64ZZ6El8/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Event Modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1deiMO70bQLJJUWgO5zDRdlBC9BP6FXH9QMQgAnfCSaA/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Distributed Serverless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/actiwerks/JOpenSpace2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomáš Janečka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Prototypovanie deskových hier + využitie AI nástrojov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/tom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1aFYv0B77kvQDiL0eKRBmywroo7iVzmJ6OZnXmlwPQN4/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavel Kříž</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 KNX, ta jediná správná domácí automatizace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/pavel-kriz-cz/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1bVry4V0QrwJmw4ZiGIGTrkI-hFaPeke71Woc_61eK8A/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavel Šimerda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Systémové programovací jazyky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/file/d/1DA2WoEE2m0ftNlCWzA_fXu60t9_CvOAD/view?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Je čas opustit AWS?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1ryH7oGEWlsbvkz2G9cNXRmw-7qwDQmy_unh9cskr_ns/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Datové struktury optimalizované pro cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1oP2ESRrVwW1D_d82H4ACDzlAooDebIRjmQ-Z9JIJNbM/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomáš Zezula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Dynamické objekty v Kotlinu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/in/zezulatomas/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/16rFLeR9TVHyDpnufA56qAyXneskjv_AJDAnf6mz-Sx0/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 Abstrakce a reprezentace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://witter.cz/@calavera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1m5UEhpDeCTzoOtDHYfAb8qh0KnKUPUxQpwzIm9vG4u4/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤 RTO nebo GTFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://witter.cz/@wvi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1nsSU1fT0ysECDCbxlT0dw-exEWUyYgPB/edit?usp=sharing&amp;ouid=104091090538791778827&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chemiX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤Deskove hry, jak na ne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">honzacerny.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.figma.com/deck/tTzlnhuKFmT0lkKrYKQn1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Petrla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎤Poletíme ke hvězdám? Pokrok v raketových motorech.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/presentation/d/1FUKB6PU6YjGb4baaBKLjWfTGAdGCWRLW/edit?usp=sharing&amp;ouid=106532318343114098414&amp;rtpof=true&amp;sd=true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pavel Tomášek</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">🎤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">Výuka informatiky na neinformatické fakultě</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3255,7 +3556,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3298,12 +3599,20 @@
       <color rgb="FFA9B7C6"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="13.5"/>
       <color rgb="FFA9B7C6"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3372,7 +3681,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3393,10 +3702,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3405,19 +3710,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3505,9 +3810,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.09"/>
@@ -4343,9 +4648,9 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="57.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="49.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="30.09"/>
@@ -4520,7 +4825,7 @@
       <c r="B11" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>276</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -4698,7 +5003,7 @@
       <c r="B22" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="1" t="s">
         <v>321</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -4754,19 +5059,19 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="5"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="5"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="5"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="5"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="5"/>
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4809,9 +5114,9 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="57.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="49.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="30.09"/>
@@ -4841,10 +5146,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>336</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -4853,7 +5158,7 @@
       <c r="D2" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>339</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -4861,16 +5166,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>341</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>343</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -4878,10 +5183,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>346</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -4890,7 +5195,7 @@
       <c r="D4" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>349</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -4898,10 +5203,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>351</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -4910,7 +5215,7 @@
       <c r="D5" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>354</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -4918,10 +5223,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>356</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -4930,7 +5235,7 @@
       <c r="D6" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>359</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -4938,10 +5243,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>361</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -4950,7 +5255,7 @@
       <c r="D7" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>364</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -4958,10 +5263,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>367</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -4978,10 +5283,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>372</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4990,7 +5295,7 @@
       <c r="D9" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>375</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -4998,10 +5303,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>377</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -5010,7 +5315,7 @@
       <c r="D10" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>380</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -5018,10 +5323,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>382</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -5030,7 +5335,7 @@
       <c r="D11" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>385</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -5038,10 +5343,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>388</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -5050,7 +5355,7 @@
       <c r="D12" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>390</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -5058,10 +5363,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>393</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -5070,7 +5375,7 @@
       <c r="D13" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>396</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -5078,10 +5383,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>399</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5090,7 +5395,7 @@
       <c r="D14" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>402</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -5098,10 +5403,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>405</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -5110,7 +5415,7 @@
       <c r="D15" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>408</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -5118,10 +5423,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>410</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -5130,7 +5435,7 @@
       <c r="D16" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>413</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -5138,10 +5443,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>416</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -5150,7 +5455,7 @@
       <c r="D17" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>419</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -5158,10 +5463,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>422</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -5170,7 +5475,7 @@
       <c r="D18" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>425</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -5178,10 +5483,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>427</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -5190,7 +5495,7 @@
       <c r="D19" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>430</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -5198,10 +5503,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>433</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -5210,7 +5515,7 @@
       <c r="D20" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>436</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -5218,10 +5523,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>439</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -5230,7 +5535,7 @@
       <c r="D21" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>442</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -5238,10 +5543,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>444</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -5250,7 +5555,7 @@
       <c r="D22" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>447</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -5258,10 +5563,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>449</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -5270,7 +5575,7 @@
       <c r="D23" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>452</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -5278,10 +5583,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>454</v>
       </c>
       <c r="C24" s="4" t="s">
@@ -5290,7 +5595,7 @@
       <c r="D24" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>457</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -5298,10 +5603,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>460</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -5310,7 +5615,7 @@
       <c r="D25" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>463</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -5318,19 +5623,19 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="5"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="5"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="5"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="5"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="5"/>
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5386,13 +5691,13 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="68.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="43.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="30.09"/>
@@ -5431,7 +5736,7 @@
       <c r="C2" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>467</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -5451,7 +5756,7 @@
       <c r="C3" s="0" t="s">
         <v>472</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>473</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -5471,10 +5776,10 @@
       <c r="C4" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>479</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -5491,10 +5796,10 @@
       <c r="C5" s="0" t="s">
         <v>482</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>484</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -5511,10 +5816,10 @@
       <c r="C6" s="0" t="s">
         <v>487</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>489</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -5531,7 +5836,7 @@
       <c r="C7" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="2" t="s">
         <v>493</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -5551,7 +5856,7 @@
       <c r="C8" s="0" t="s">
         <v>497</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="2" t="s">
         <v>498</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -5571,7 +5876,7 @@
       <c r="C9" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="2" t="s">
         <v>504</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -5591,10 +5896,10 @@
       <c r="C10" s="0" t="s">
         <v>509</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>511</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -5611,7 +5916,7 @@
       <c r="C11" s="0" t="s">
         <v>514</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>515</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -5631,10 +5936,10 @@
       <c r="C12" s="0" t="s">
         <v>520</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>522</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -5651,10 +5956,10 @@
       <c r="C13" s="0" t="s">
         <v>525</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>527</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -5672,7 +5977,7 @@
         <v>530</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>531</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -5689,7 +5994,7 @@
       <c r="C15" s="0" t="s">
         <v>534</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="2" t="s">
         <v>535</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -5709,7 +6014,7 @@
       <c r="C16" s="0" t="s">
         <v>539</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="2" t="s">
         <v>540</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -5726,13 +6031,13 @@
       <c r="B17" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="3" t="s">
         <v>547</v>
       </c>
@@ -5747,7 +6052,7 @@
       <c r="C18" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="2" t="s">
         <v>551</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -5767,7 +6072,7 @@
       <c r="C19" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="2" t="s">
         <v>556</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -5784,13 +6089,13 @@
       <c r="B20" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>561</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>563</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -5807,7 +6112,7 @@
       <c r="C21" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="2" t="s">
         <v>568</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -5827,7 +6132,7 @@
       <c r="C22" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="2" t="s">
         <v>573</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -5844,13 +6149,13 @@
       <c r="B23" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="2"/>
       <c r="F23" s="3" t="s">
         <v>580</v>
       </c>
@@ -5865,10 +6170,10 @@
       <c r="C24" s="0" t="s">
         <v>583</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>585</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -5885,7 +6190,7 @@
       <c r="C25" s="0" t="s">
         <v>589</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
         <v>590</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -5905,7 +6210,7 @@
       <c r="C26" s="0" t="s">
         <v>595</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="2" t="s">
         <v>596</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -5925,7 +6230,7 @@
       <c r="C27" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="2" t="s">
         <v>601</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -5945,10 +6250,10 @@
       <c r="C28" s="0" t="s">
         <v>605</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="3" t="s">
         <v>607</v>
       </c>
@@ -5963,7 +6268,7 @@
       <c r="C29" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="2" t="s">
         <v>609</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -5983,7 +6288,7 @@
       <c r="C30" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="2" t="s">
         <v>613</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -6003,7 +6308,7 @@
       <c r="C31" s="0" t="s">
         <v>618</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="2" t="s">
         <v>619</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -6023,7 +6328,7 @@
       <c r="C32" s="0" t="s">
         <v>624</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="2" t="s">
         <v>625</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -6043,7 +6348,7 @@
       <c r="C33" s="0" t="s">
         <v>629</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="2" t="s">
         <v>630</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -6063,7 +6368,7 @@
       <c r="C34" s="0" t="s">
         <v>635</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="2" t="s">
         <v>636</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -6083,7 +6388,7 @@
       <c r="C35" s="0" t="s">
         <v>640</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="2" t="s">
         <v>641</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -6103,7 +6408,7 @@
       <c r="C36" s="0" t="s">
         <v>645</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="2" t="s">
         <v>646</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -6123,7 +6428,7 @@
       <c r="C37" s="0" t="s">
         <v>651</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="2" t="s">
         <v>652</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -6141,7 +6446,7 @@
         <v>655</v>
       </c>
       <c r="C38" s="0"/>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="2" t="s">
         <v>656</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -6161,7 +6466,7 @@
       <c r="C39" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="2" t="s">
         <v>661</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -6181,7 +6486,7 @@
       <c r="C40" s="0" t="s">
         <v>666</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="2" t="s">
         <v>667</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -6201,7 +6506,7 @@
       <c r="C41" s="0" t="s">
         <v>671</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="2" t="s">
         <v>672</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -6221,7 +6526,7 @@
       <c r="C42" s="0" t="s">
         <v>676</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="2" t="s">
         <v>677</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -6277,4 +6582,545 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="108.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="56.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>696</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>762</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>772</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="https://docs.google.com/presentation/d/1vAPAkLOSTeKivvjCpFT8fGvTJnNMqksJ4q5yKX8FkQ0/edit?usp=sharing"/>
+    <hyperlink ref="E4" r:id="rId2" display="https://docs.google.com/presentation/d/1etgJfsgDy_LR3eNW1ArESDER-lq1Fasqyx7TH6Tcmog/edit?usp=sharing"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://www.linkedin.com/in/milanlempera/"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://docs.google.com/presentation/d/1DjGQOEuifkzH4lVNIA1wUB5S0-N43iNjK8XBSdCIZ28/edit?usp=sharing"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://www.linkedin.com/in/miloshavranek"/>
+    <hyperlink ref="E6" r:id="rId6" display="https://docs.google.com/presentation/d/1e2b5doe5V0wi0DlxOmBCOKHLKwsu4Q6riUDtTpqEX7o/edit"/>
+    <hyperlink ref="C7" r:id="rId7" display="https://cz.linkedin.com/in/jirkapinkas"/>
+    <hyperlink ref="E7" r:id="rId8" display="https://docs.google.com/presentation/d/1GtbMVHhNK7DrKEw4cKfzkKqt7AKRV2OWIUK-j-dEXPY/edit?usp=sharing"/>
+    <hyperlink ref="E8" r:id="rId9" display="https://drive.google.com/file/d/1Y0jf3tYs3yv6qJ__QW7WA8orRGsQeyf9/view?usp=drive_link"/>
+    <hyperlink ref="E9" r:id="rId10" display="https://docs.google.com/presentation/d/1xukBVbrc6piYvDD_lllap9GmMxBucU4n4plrO7b5Two/edit?usp=sharing"/>
+    <hyperlink ref="C10" r:id="rId11" display="https://www.vojtechruzicka.com/about/"/>
+    <hyperlink ref="E10" r:id="rId12" location="slide=id.g3042c971e74_0_0" display="https://docs.google.com/presentation/d/1V0S-XLpO79DJUz9FeOLH2YzY7D5eFlNiZSiq4mEJaJA/edit#slide=id.g3042c971e74_0_0"/>
+    <hyperlink ref="C11" r:id="rId13" display="https://www.linkedin.com/in/jannovotny/"/>
+    <hyperlink ref="E11" r:id="rId14" display="https://novoj.github.io/reveal.js/jopenspace2024.html"/>
+    <hyperlink ref="E13" r:id="rId15" location="slide=id.g2d3e48ff1ef_0_0" display="https://docs.google.com/presentation/d/1gw9-1-7JpieulzRNrkte2SnQtOwsFaYndec0jEomNsk/edit#slide=id.g2d3e48ff1ef_0_0"/>
+    <hyperlink ref="C14" r:id="rId16" display="https://www.linkedin.com/in/leosprikryl/"/>
+    <hyperlink ref="E14" r:id="rId17" display="https://docs.google.com/presentation/d/1xk2bZjr_H16P_NBaKTibx-E1dODgjiNG5WSagivHtmQ/edit?usp=sharing"/>
+    <hyperlink ref="E15" r:id="rId18" location="slide=id.p" display="https://docs.google.com/presentation/d/1YzXB9UEiNi6RIlDg987zW6ah0sgjNYYLtuUZ-S7N5S0/edit#slide=id.p"/>
+    <hyperlink ref="E16" r:id="rId19" display="https://github.com/bugs84/idea-debugging"/>
+    <hyperlink ref="C18" r:id="rId20" display="https://www.linkedin.com/in/vaclav-stolin/"/>
+    <hyperlink ref="E18" r:id="rId21" display="https://docs.google.com/presentation/d/1Dz3IoOa8e8ENW-s3wzTjO3lgnoDL80Ua9Sip1gJl1xs/edit?usp=drivesdk"/>
+    <hyperlink ref="C19" r:id="rId22" display="https://mastodon.social/@dondcz"/>
+    <hyperlink ref="E19" r:id="rId23" display="https://docs.google.com/presentation/d/1-FaHoEOYTGCGuU-N3a8Kv5Zs7-cHMHgWWuueAtdNles/edit"/>
+    <hyperlink ref="C20" r:id="rId24" display="https://www.linkedin.com/in/vitaplsek"/>
+    <hyperlink ref="E20" r:id="rId25" display="https://drive.google.com/file/d/1lpEmMXVCthu0ryCtH4RNhIxSfHZdD9dR/view?usp=sharing"/>
+    <hyperlink ref="E21" r:id="rId26" display="https://docs.google.com/presentation/d/1Mn2zGT3l1hjI-unTH6ch7dGVGUJ8hg_K/edit?usp=sharing&amp;ouid=116470056523174499937&amp;rtpof=true&amp;sd=true"/>
+    <hyperlink ref="C22" r:id="rId27" display="https://sika.io/"/>
+    <hyperlink ref="E22" r:id="rId28" display="https://docs.google.com/presentation/d/1zeEhah2i5J5RGENYm9ieA91JhK5lD3lwWQc0RU_Pa28/edit"/>
+    <hyperlink ref="C23" r:id="rId29" display="https://www.linkedin.com/in/vladimirorany/"/>
+    <hyperlink ref="E23" r:id="rId30" display="https://docs.google.com/presentation/d/1ZkpR4FWX_VRYsC-U6jDXRV5lwcpXd9ietQp64ZZ6El8/edit?usp=sharing"/>
+    <hyperlink ref="C24" r:id="rId31" display="https://www.linkedin.com/in/marianschubert/"/>
+    <hyperlink ref="E24" r:id="rId32" display="https://docs.google.com/presentation/d/1deiMO70bQLJJUWgO5zDRdlBC9BP6FXH9QMQgAnfCSaA/edit?usp=sharing"/>
+    <hyperlink ref="E25" r:id="rId33" display="https://github.com/actiwerks/JOpenSpace2024"/>
+    <hyperlink ref="C26" r:id="rId34" display="https://www.linkedin.com/in/tom"/>
+    <hyperlink ref="E26" r:id="rId35" display="https://docs.google.com/presentation/d/1aFYv0B77kvQDiL0eKRBmywroo7iVzmJ6OZnXmlwPQN4/edit?usp=sharing"/>
+    <hyperlink ref="C27" r:id="rId36" display="https://www.linkedin.com/in/pavel-kriz-cz/"/>
+    <hyperlink ref="E27" r:id="rId37" display="https://docs.google.com/presentation/d/1bVry4V0QrwJmw4ZiGIGTrkI-hFaPeke71Woc_61eK8A/edit?usp=sharing"/>
+    <hyperlink ref="E28" r:id="rId38" display="https://drive.google.com/file/d/1DA2WoEE2m0ftNlCWzA_fXu60t9_CvOAD/view?usp=sharing"/>
+    <hyperlink ref="E29" r:id="rId39" display="https://docs.google.com/presentation/d/1ryH7oGEWlsbvkz2G9cNXRmw-7qwDQmy_unh9cskr_ns/edit?usp=sharing"/>
+    <hyperlink ref="E30" r:id="rId40" display="https://docs.google.com/presentation/d/1oP2ESRrVwW1D_d82H4ACDzlAooDebIRjmQ-Z9JIJNbM/edit?usp=sharing"/>
+    <hyperlink ref="C31" r:id="rId41" display="https://www.linkedin.com/in/zezulatomas/"/>
+    <hyperlink ref="E31" r:id="rId42" display="https://docs.google.com/presentation/d/16rFLeR9TVHyDpnufA56qAyXneskjv_AJDAnf6mz-Sx0/edit?usp=sharing"/>
+    <hyperlink ref="C32" r:id="rId43" display="https://witter.cz/@calavera"/>
+    <hyperlink ref="E32" r:id="rId44" display="https://docs.google.com/presentation/d/1m5UEhpDeCTzoOtDHYfAb8qh0KnKUPUxQpwzIm9vG4u4/edit?usp=sharing"/>
+    <hyperlink ref="E33" r:id="rId45" display="https://docs.google.com/presentation/d/1nsSU1fT0ysECDCbxlT0dw-exEWUyYgPB/edit?usp=sharing&amp;ouid=104091090538791778827&amp;rtpof=true&amp;sd=true"/>
+    <hyperlink ref="C34" r:id="rId46" display="honzacerny.com"/>
+    <hyperlink ref="E34" r:id="rId47" display="https://www.figma.com/deck/tTzlnhuKFmT0lkKrYKQn1G"/>
+    <hyperlink ref="E35" r:id="rId48" display="https://docs.google.com/presentation/d/1FUKB6PU6YjGb4baaBKLjWfTGAdGCWRLW/edit?usp=sharing&amp;ouid=106532318343114098414&amp;rtpof=true&amp;sd=true"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>